<commit_message>
Hotkey agregados, queda agregar la fecha de cierre y enviar el correo
</commit_message>
<xml_diff>
--- a/Datos para oportunidades CRM.xlsx
+++ b/Datos para oportunidades CRM.xlsx
@@ -172,9 +172,1353 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1906">
+  <x:cellStyleXfs count="2354">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="6" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">

</xml_diff>